<commit_message>
completed code for data driven feature
</commit_message>
<xml_diff>
--- a/TestAssignment/cityNames.xlsx
+++ b/TestAssignment/cityNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronit\Desktop\GitHub\testvagrant-test\TestAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6191BCB-FBCA-4AAC-A03D-49A04D76438A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2327C6C-D6DB-4942-8CCE-2EA928312FF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>CityName</t>
   </si>
@@ -33,10 +33,22 @@
     <t>cityOnMap</t>
   </si>
   <si>
-    <t xml:space="preserve"> Kanpur</t>
-  </si>
-  <si>
-    <t>Kanpur</t>
+    <t xml:space="preserve"> Ajmer</t>
+  </si>
+  <si>
+    <t>Ajmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alwar</t>
+  </si>
+  <si>
+    <t>Alwar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bhilai</t>
+  </si>
+  <si>
+    <t>Bhilai</t>
   </si>
 </sst>
 </file>
@@ -354,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -381,6 +393,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>